<commit_message>
run one more PARAFAC sample
</commit_message>
<xml_diff>
--- a/data/DOM-indices_processing/PARAFAC/Results_ELA.xlsx
+++ b/data/DOM-indices_processing/PARAFAC/Results_ELA.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://trentu-my.sharepoint.com/personal/sandraklemet_trentu_ca/Documents/Documents/Etudes/Trent/Xenopoulos lab/Projects/11-DOC-ELA_animal-excretion/data/DOM-indices_processing/PARAFAC/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="146" documentId="11_A8C902C99ADF99B137553021C155FE035930B61D" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{80F351A6-099F-41EC-85E8-04FDB13C5DB2}"/>
+  <xr:revisionPtr revIDLastSave="157" documentId="11_A8C902C99ADF99B137553021C155FE035930B61D" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{EA25C8DE-F775-4FE9-83CE-BCF69F29526A}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView minimized="1" xWindow="1750" yWindow="2200" windowWidth="14580" windowHeight="7400" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="FMax" sheetId="2" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="308" uniqueCount="214">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="311" uniqueCount="216">
   <si>
     <t>C1</t>
   </si>
@@ -679,20 +679,32 @@
     <t>terrible</t>
   </si>
   <si>
-    <t>try July 1st 3m</t>
-  </si>
-  <si>
     <t>check readings on spec</t>
+  </si>
+  <si>
+    <t>PARAFAC_099</t>
+  </si>
+  <si>
+    <t>L114JULY122_corr.csv</t>
+  </si>
+  <si>
+    <t>used this one instead of the one above from June 10th</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -742,12 +754,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -763,6 +776,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1028,10 +1045,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:L99"/>
+  <dimension ref="A1:L100"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A67" workbookViewId="0">
-      <selection activeCell="P78" sqref="P78"/>
+    <sheetView tabSelected="1" topLeftCell="A89" workbookViewId="0">
+      <selection activeCell="L94" sqref="L94"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -4119,9 +4136,7 @@
       <c r="K88">
         <v>1.2964859507271467</v>
       </c>
-      <c r="L88" s="4" t="s">
-        <v>212</v>
-      </c>
+      <c r="L88" s="5"/>
     </row>
     <row r="89" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A89" s="2" t="s">
@@ -4158,7 +4173,7 @@
         <v>0.21290036500415715</v>
       </c>
       <c r="L89" s="4" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
     </row>
     <row r="90" spans="1:12" x14ac:dyDescent="0.35">
@@ -4300,6 +4315,9 @@
       <c r="K93">
         <v>0.24493694033896624</v>
       </c>
+      <c r="L93" t="s">
+        <v>215</v>
+      </c>
     </row>
     <row r="94" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A94" t="s">
@@ -4476,7 +4494,7 @@
         <v>0.20833141198434765</v>
       </c>
       <c r="L98" s="4" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
     </row>
     <row r="99" spans="1:12" x14ac:dyDescent="0.35">
@@ -4512,6 +4530,41 @@
       </c>
       <c r="K99">
         <v>0.14365261711755314</v>
+      </c>
+    </row>
+    <row r="100" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A100" s="5" t="s">
+        <v>214</v>
+      </c>
+      <c r="B100" t="s">
+        <v>213</v>
+      </c>
+      <c r="C100">
+        <v>-0.05</v>
+      </c>
+      <c r="D100" t="s">
+        <v>207</v>
+      </c>
+      <c r="E100">
+        <v>0.49755234777302848</v>
+      </c>
+      <c r="F100">
+        <v>0.73122499976708988</v>
+      </c>
+      <c r="G100">
+        <v>0.43763335259661901</v>
+      </c>
+      <c r="H100">
+        <v>0.10791857827164017</v>
+      </c>
+      <c r="I100">
+        <v>0.1444948942843563</v>
+      </c>
+      <c r="J100">
+        <v>0</v>
+      </c>
+      <c r="K100">
+        <v>0.27149173755646527</v>
       </c>
     </row>
   </sheetData>
@@ -4520,6 +4573,7 @@
       <sortCondition ref="A1:A99"/>
     </sortState>
   </autoFilter>
+  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>

<commit_message>
modified code for DOM excretion rates processing
</commit_message>
<xml_diff>
--- a/data/DOM-indices_processing/PARAFAC/Results_ELA.xlsx
+++ b/data/DOM-indices_processing/PARAFAC/Results_ELA.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://trentu-my.sharepoint.com/personal/sandraklemet_trentu_ca/Documents/Documents/Etudes/Trent/Xenopoulos lab/Projects/11-DOC-ELA_animal-excretion/data/DOM-indices_processing/PARAFAC/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="157" documentId="11_A8C902C99ADF99B137553021C155FE035930B61D" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{EA25C8DE-F775-4FE9-83CE-BCF69F29526A}"/>
+  <xr:revisionPtr revIDLastSave="158" documentId="11_A8C902C99ADF99B137553021C155FE035930B61D" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{0A22B567-D3B9-475B-BA59-09D449A9B7E6}"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="1750" yWindow="2200" windowWidth="14580" windowHeight="7400" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="FMax" sheetId="2" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="311" uniqueCount="216">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="312" uniqueCount="217">
   <si>
     <t>C1</t>
   </si>
@@ -689,6 +689,9 @@
   </si>
   <si>
     <t>used this one instead of the one above from June 10th</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
   </si>
 </sst>
 </file>
@@ -754,13 +757,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -776,10 +778,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1047,8 +1045,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L100"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A89" workbookViewId="0">
-      <selection activeCell="L94" sqref="L94"/>
+    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
+      <selection activeCell="D40" sqref="D40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3297,7 +3295,7 @@
         <v>0.25723052150893871</v>
       </c>
     </row>
-    <row r="65" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A65" s="2" t="s">
         <v>135</v>
       </c>
@@ -3332,7 +3330,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="66" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A66" s="2" t="s">
         <v>137</v>
       </c>
@@ -3367,7 +3365,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="67" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A67" s="3" t="s">
         <v>139</v>
       </c>
@@ -3402,7 +3400,7 @@
         <v>0.17548792393048532</v>
       </c>
     </row>
-    <row r="68" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A68" t="s">
         <v>141</v>
       </c>
@@ -3437,7 +3435,7 @@
         <v>0.37057582503842845</v>
       </c>
     </row>
-    <row r="69" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A69" t="s">
         <v>143</v>
       </c>
@@ -3472,7 +3470,7 @@
         <v>0.21272072750342799</v>
       </c>
     </row>
-    <row r="70" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A70" s="1" t="s">
         <v>145</v>
       </c>
@@ -3507,7 +3505,7 @@
         <v>0.40606582730602797</v>
       </c>
     </row>
-    <row r="71" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A71" t="s">
         <v>147</v>
       </c>
@@ -3542,7 +3540,7 @@
         <v>0.21261890814487772</v>
       </c>
     </row>
-    <row r="72" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A72" s="3" t="s">
         <v>149</v>
       </c>
@@ -3577,7 +3575,7 @@
         <v>0.13121624834166515</v>
       </c>
     </row>
-    <row r="73" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A73" s="3" t="s">
         <v>151</v>
       </c>
@@ -3612,7 +3610,7 @@
         <v>0.1552572598028733</v>
       </c>
     </row>
-    <row r="74" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A74" s="3" t="s">
         <v>153</v>
       </c>
@@ -3647,7 +3645,7 @@
         <v>0.14286595686854212</v>
       </c>
     </row>
-    <row r="75" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A75" s="3" t="s">
         <v>155</v>
       </c>
@@ -3682,7 +3680,7 @@
         <v>0.13724297622970585</v>
       </c>
     </row>
-    <row r="76" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A76" s="3" t="s">
         <v>157</v>
       </c>
@@ -3717,7 +3715,7 @@
         <v>0.10024202338185051</v>
       </c>
     </row>
-    <row r="77" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A77" s="3" t="s">
         <v>159</v>
       </c>
@@ -3752,7 +3750,7 @@
         <v>0.14215050863502623</v>
       </c>
     </row>
-    <row r="78" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A78" s="3" t="s">
         <v>161</v>
       </c>
@@ -3787,7 +3785,7 @@
         <v>0.14362593421463959</v>
       </c>
     </row>
-    <row r="79" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A79" s="3" t="s">
         <v>163</v>
       </c>
@@ -3822,7 +3820,7 @@
         <v>0.22587812165894819</v>
       </c>
     </row>
-    <row r="80" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="80" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A80" s="3" t="s">
         <v>165</v>
       </c>
@@ -3855,6 +3853,9 @@
       </c>
       <c r="K80">
         <v>0.21744927081250232</v>
+      </c>
+      <c r="L80" t="s">
+        <v>216</v>
       </c>
     </row>
     <row r="81" spans="1:12" x14ac:dyDescent="0.35">
@@ -4136,7 +4137,6 @@
       <c r="K88">
         <v>1.2964859507271467</v>
       </c>
-      <c r="L88" s="5"/>
     </row>
     <row r="89" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A89" s="2" t="s">
@@ -4533,7 +4533,7 @@
       </c>
     </row>
     <row r="100" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A100" s="5" t="s">
+      <c r="A100" t="s">
         <v>214</v>
       </c>
       <c r="B100" t="s">

</xml_diff>